<commit_message>
Grandes olhos, nasce uma estrela added
</commit_message>
<xml_diff>
--- a/Relação.xlsx
+++ b/Relação.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="82">
   <si>
     <t>Nome</t>
   </si>
@@ -108,6 +108,9 @@
     <t>Sniper Américano</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Um lugar Silencioso</t>
   </si>
   <si>
@@ -240,9 +243,6 @@
     <t>Amantes Eternos</t>
   </si>
   <si>
-    <t>Pen.</t>
-  </si>
-  <si>
     <t>Clube da luta</t>
   </si>
   <si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Grandes olhos</t>
+  </si>
+  <si>
+    <t>Nasce uma estrla</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF7030A0"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -362,7 +368,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -518,8 +524,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D72" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:D72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D75" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:D75">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Filme"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:D65">
     <sortCondition ref="D1:D65"/>
   </sortState>
@@ -820,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -878,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -892,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -906,7 +918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -920,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -934,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1075,9 +1087,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1089,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -1103,9 +1115,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -1117,9 +1129,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
@@ -1131,9 +1143,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
@@ -1145,9 +1157,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -1159,9 +1171,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
@@ -1173,9 +1185,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>18</v>
@@ -1187,9 +1199,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>18</v>
@@ -1201,9 +1213,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
@@ -1215,9 +1227,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>18</v>
@@ -1229,9 +1241,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>18</v>
@@ -1243,9 +1255,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>18</v>
@@ -1257,9 +1269,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>18</v>
@@ -1271,9 +1283,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>18</v>
@@ -1285,9 +1297,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>18</v>
@@ -1299,9 +1311,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>18</v>
@@ -1313,9 +1325,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>18</v>
@@ -1327,9 +1339,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>18</v>
@@ -1427,7 +1439,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
@@ -1441,7 +1453,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>5</v>
@@ -1455,7 +1467,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
@@ -1469,21 +1481,21 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="1">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
@@ -1497,7 +1509,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
@@ -1511,7 +1523,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -1525,7 +1537,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
@@ -1539,7 +1551,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
@@ -1553,7 +1565,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>5</v>
@@ -1567,7 +1579,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>5</v>
@@ -1581,7 +1593,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>5</v>
@@ -1595,7 +1607,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
@@ -1609,7 +1621,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
@@ -1623,7 +1635,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
@@ -1637,7 +1649,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>5</v>
@@ -1665,7 +1677,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
@@ -1679,7 +1691,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
@@ -1693,7 +1705,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>5</v>
@@ -1707,7 +1719,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
@@ -1721,7 +1733,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
@@ -1735,7 +1747,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
@@ -1749,7 +1761,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
@@ -1763,7 +1775,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
@@ -1777,7 +1789,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
@@ -1791,7 +1803,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
@@ -1825,28 +1837,57 @@
         <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="D71" s="2">
         <v>4</v>
       </c>
     </row>
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C72">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="P">
+  <conditionalFormatting sqref="C2:C75">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A72">
-    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
+  <conditionalFormatting sqref="A1:A75">
+    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"CC"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Hércules and Diamante de Sangue added
</commit_message>
<xml_diff>
--- a/Relação.xlsx
+++ b/Relação.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1C1302-9B56-4798-9BA4-871229BB468A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF56DF06-FAEF-428C-B4AE-70FFB0139598}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="94">
   <si>
     <t>Nome</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>O homem invisível</t>
+  </si>
+  <si>
+    <t>Hércules</t>
+  </si>
+  <si>
+    <t>Diamante de sangue</t>
   </si>
 </sst>
 </file>
@@ -381,21 +387,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -584,8 +576,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:E84" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:E84" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:E85" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:E85" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="Filme"/>
@@ -596,11 +588,11 @@
     <sortCondition ref="D1:D65"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tipo " dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Host" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{21B0E347-E6FA-4E51-BC19-11AFEF935054}" name="Data" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tipo " dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Host" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{21B0E347-E6FA-4E51-BC19-11AFEF935054}" name="Data" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -927,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2200,28 +2192,55 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="7"/>
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="6">
+        <v>5</v>
+      </c>
+      <c r="E84" s="7">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="6">
+        <v>5</v>
+      </c>
+      <c r="E85" s="7">
+        <v>44225</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C84">
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="P">
+  <conditionalFormatting sqref="C2:C85">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A84">
-    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+  <conditionalFormatting sqref="A1:A85">
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"CC"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
A rede social added
</commit_message>
<xml_diff>
--- a/Relação.xlsx
+++ b/Relação.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528BEF46-BF94-47C6-9164-C16F17DD74FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD2929E-4297-41B4-BF4B-22B86B591CC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7110" yWindow="2580" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="104">
   <si>
     <t>Nome</t>
   </si>
@@ -212,9 +223,6 @@
     <t>V de Vingança</t>
   </si>
   <si>
-    <t>Eu Robô</t>
-  </si>
-  <si>
     <t>Coringa</t>
   </si>
   <si>
@@ -254,52 +262,82 @@
     <t>As sufragistas</t>
   </si>
   <si>
+    <t>Grandes olhos</t>
+  </si>
+  <si>
+    <t>Nasce uma estrla</t>
+  </si>
+  <si>
+    <t>Mad Max - Estrada da Fúria</t>
+  </si>
+  <si>
+    <t>Maze Runner - Correr ou Morrer</t>
+  </si>
+  <si>
+    <t>Wall-e</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Maze Runner - Prova de fogo</t>
+  </si>
+  <si>
+    <t>Maze Runner - A cura mortal</t>
+  </si>
+  <si>
+    <t>O auto da Conpadecida</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>Prenda-me se for capaz</t>
+  </si>
+  <si>
+    <t>O homem invisível</t>
+  </si>
+  <si>
+    <t>Hércules</t>
+  </si>
+  <si>
+    <t>Diamante de sangue</t>
+  </si>
+  <si>
+    <t>Chappie</t>
+  </si>
+  <si>
+    <t>Star Wars - A assenção de Sky Walker</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Peso MB</t>
+  </si>
+  <si>
+    <t>A fuga das galinhas</t>
+  </si>
+  <si>
+    <t>Eu, Robô</t>
+  </si>
+  <si>
+    <t>Não sei</t>
+  </si>
+  <si>
+    <t>A rede social</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Grandes olhos</t>
-  </si>
-  <si>
-    <t>Nasce uma estrla</t>
-  </si>
-  <si>
-    <t>Mad Max - Estrada da Fúria</t>
-  </si>
-  <si>
-    <t>Maze Runner - Correr ou Morrer</t>
-  </si>
-  <si>
-    <t>Wall-e</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Maze Runner - Prova de fogo</t>
-  </si>
-  <si>
-    <t>Maze Runner - A cura mortal</t>
-  </si>
-  <si>
-    <t>O auto da Conpadecida</t>
-  </si>
-  <si>
-    <t>Titanic</t>
-  </si>
-  <si>
-    <t>Prenda-me se for capaz</t>
-  </si>
-  <si>
-    <t>O homem invisível</t>
-  </si>
-  <si>
-    <t>Hércules</t>
-  </si>
-  <si>
-    <t>Diamante de sangue</t>
-  </si>
-  <si>
-    <t>Chappie</t>
+    <t>Coraline</t>
+  </si>
+  <si>
+    <t>Sinais</t>
+  </si>
+  <si>
+    <t>Tá dando onda</t>
   </si>
 </sst>
 </file>
@@ -363,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -386,15 +424,240 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -533,32 +796,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -579,23 +832,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:E86" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:E86" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:F92" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:F91" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="1">
-      <filters>
+      <filters blank="1">
         <filter val="Filme"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
-    <sortCondition ref="D1:D65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F87">
+    <sortCondition ref="D1:D87"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tipo " dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Host" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{21B0E347-E6FA-4E51-BC19-11AFEF935054}" name="Data" dataDxfId="2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tipo " dataDxfId="26" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status" dataDxfId="25" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Host" dataDxfId="24" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8822ACAF-798B-4D07-9264-792FB268BD2D}" name="Peso MB" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{21B0E347-E6FA-4E51-BC19-11AFEF935054}" name="Data" dataDxfId="22" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -922,23 +1181,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -951,61 +1211,70 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1070</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>683</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -1013,14 +1282,14 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -1028,29 +1297,32 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="8">
+        <v>950</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
@@ -1058,42 +1330,42 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -1104,11 +1376,11 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -1119,11 +1391,11 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1134,11 +1406,11 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -1149,56 +1421,60 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="5">
+        <v>43789</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1209,11 +1485,12 @@
       <c r="D18" s="1">
         <v>2</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
@@ -1224,11 +1501,12 @@
       <c r="D19" s="1">
         <v>2</v>
       </c>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -1239,11 +1517,12 @@
       <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
@@ -1254,11 +1533,12 @@
       <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
@@ -1269,11 +1549,12 @@
       <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -1284,11 +1565,12 @@
       <c r="D23" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
@@ -1299,11 +1581,12 @@
       <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>18</v>
@@ -1314,11 +1597,12 @@
       <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>18</v>
@@ -1329,11 +1613,12 @@
       <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>18</v>
@@ -1344,11 +1629,12 @@
       <c r="D27" s="1">
         <v>2</v>
       </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="1"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>18</v>
@@ -1359,11 +1645,12 @@
       <c r="D28" s="1">
         <v>2</v>
       </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="1"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>18</v>
@@ -1374,11 +1661,12 @@
       <c r="D29" s="1">
         <v>2</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="1"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>18</v>
@@ -1389,11 +1677,12 @@
       <c r="D30" s="1">
         <v>2</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="1"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>18</v>
@@ -1404,11 +1693,12 @@
       <c r="D31" s="1">
         <v>2</v>
       </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="1"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>18</v>
@@ -1419,11 +1709,12 @@
       <c r="D32" s="1">
         <v>2</v>
       </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>18</v>
@@ -1434,11 +1725,12 @@
       <c r="D33" s="1">
         <v>2</v>
       </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>18</v>
@@ -1449,26 +1741,29 @@
       <c r="D34" s="1">
         <v>2</v>
       </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
       </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="5">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>18</v>
@@ -1477,73 +1772,78 @@
         <v>8</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
-      </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="1">
-        <v>2</v>
-      </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2</v>
-      </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2</v>
-      </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="1">
-        <v>2</v>
-      </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>5</v>
@@ -1554,86 +1854,111 @@
       <c r="D41" s="1">
         <v>2</v>
       </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="8">
+        <v>1150</v>
+      </c>
+      <c r="F41" s="5">
+        <v>43945</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1">
         <v>2</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="8">
+        <v>1020</v>
+      </c>
+      <c r="F42" s="5">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="D43" s="1">
         <v>2</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="5">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="5">
+        <v>43883</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="8">
+        <v>868</v>
+      </c>
+      <c r="F45" s="5">
+        <v>43888</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="6">
+        <v>2</v>
+      </c>
+      <c r="E46" s="11">
+        <v>1360</v>
+      </c>
+      <c r="F46" s="7">
+        <v>44233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="1">
-        <v>3</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="1">
-        <v>3</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
@@ -1644,11 +1969,16 @@
       <c r="D47" s="1">
         <v>3</v>
       </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="8">
+        <v>732</v>
+      </c>
+      <c r="F47" s="5">
+        <v>44002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
@@ -1659,11 +1989,16 @@
       <c r="D48" s="1">
         <v>3</v>
       </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="8">
+        <v>1010</v>
+      </c>
+      <c r="F48" s="5">
+        <v>44002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -1674,11 +2009,16 @@
       <c r="D49" s="1">
         <v>3</v>
       </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="8">
+        <v>815</v>
+      </c>
+      <c r="F49" s="5">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
@@ -1689,11 +2029,13 @@
       <c r="D50" s="1">
         <v>3</v>
       </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="5">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
@@ -1704,11 +2046,16 @@
       <c r="D51" s="1">
         <v>3</v>
       </c>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="8">
+        <v>1130</v>
+      </c>
+      <c r="F51" s="5">
+        <v>44003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>5</v>
@@ -1719,56 +2066,71 @@
       <c r="D52" s="1">
         <v>3</v>
       </c>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="8">
+        <v>967</v>
+      </c>
+      <c r="F52" s="5">
+        <v>44020</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D53" s="1">
         <v>3</v>
       </c>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="8">
+        <v>811</v>
+      </c>
+      <c r="F53" s="5">
+        <v>44188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="D54" s="1">
         <v>3</v>
       </c>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="8">
+        <v>1110</v>
+      </c>
+      <c r="F54" s="5">
+        <v>44002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="1">
-        <v>3</v>
-      </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
@@ -1779,26 +2141,34 @@
       <c r="D56" s="1">
         <v>3</v>
       </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="8">
+        <v>980</v>
+      </c>
+      <c r="F56" s="5">
+        <v>44018</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="1">
-        <v>3</v>
-      </c>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="8">
+        <v>1060</v>
+      </c>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>5</v>
@@ -1809,56 +2179,73 @@
       <c r="D58" s="1">
         <v>3</v>
       </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="F58" s="5">
+        <v>44018</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3</v>
+      </c>
+      <c r="E59" s="8">
+        <v>1400</v>
+      </c>
+      <c r="F59" s="5">
+        <v>44002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3</v>
+      </c>
+      <c r="E60" s="8">
+        <v>798</v>
+      </c>
+      <c r="F60" s="5">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="1">
+        <v>3</v>
+      </c>
+      <c r="E61" s="8">
+        <v>793</v>
+      </c>
+      <c r="F61" s="5">
+        <v>44003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>1917</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="2">
-        <v>4</v>
-      </c>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="2">
-        <v>4</v>
-      </c>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>5</v>
@@ -1869,56 +2256,74 @@
       <c r="D62" s="2">
         <v>4</v>
       </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="9">
+        <v>1140</v>
+      </c>
+      <c r="F62" s="5">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>6</v>
+      <c r="C63" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D63" s="2">
         <v>4</v>
       </c>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>6</v>
+      <c r="E63" s="9">
+        <v>2150</v>
+      </c>
+      <c r="F63" s="5">
+        <v>44176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D64" s="2">
         <v>4</v>
       </c>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="9">
+        <v>1160</v>
+      </c>
+      <c r="F64" s="5">
+        <v>44188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D65" s="2">
         <v>4</v>
       </c>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="9"/>
+      <c r="F65" s="5">
+        <v>44174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
@@ -1929,11 +2334,19 @@
       <c r="D66" s="2">
         <v>4</v>
       </c>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="9">
+        <v>957</v>
+      </c>
+      <c r="F66" s="5">
+        <v>44142</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
@@ -1944,325 +2357,512 @@
       <c r="D67" s="2">
         <v>4</v>
       </c>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="9">
+        <v>980</v>
+      </c>
+      <c r="F67" s="5">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="2">
-        <v>4</v>
-      </c>
-      <c r="E68" s="5"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E68" s="9">
+        <v>895</v>
+      </c>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>8</v>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D69" s="2">
         <v>4</v>
       </c>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>75</v>
+      <c r="E69" s="9">
+        <v>926</v>
+      </c>
+      <c r="F69" s="5">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="D70" s="2">
         <v>4</v>
       </c>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="E70" s="9">
+        <v>769</v>
+      </c>
+      <c r="F70" s="5">
+        <v>44130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="2">
         <v>4</v>
       </c>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="9">
+        <v>907</v>
+      </c>
+      <c r="F71" s="5">
+        <v>44170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2">
+        <v>4</v>
+      </c>
+      <c r="E72" s="9">
+        <v>1050</v>
+      </c>
+      <c r="F72" s="5">
+        <v>44173</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1">
+        <v>4</v>
+      </c>
+      <c r="E73" s="8">
+        <v>1050</v>
+      </c>
+      <c r="F73" s="5">
+        <v>44187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="2">
+        <v>4</v>
+      </c>
+      <c r="E74" s="9">
+        <v>697</v>
+      </c>
+      <c r="F74" s="5">
+        <v>44174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1">
+        <v>5</v>
+      </c>
+      <c r="E75" s="8">
+        <v>696</v>
+      </c>
+      <c r="F75" s="5">
+        <v>44232</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="6">
+        <v>5</v>
+      </c>
+      <c r="E76" s="11">
+        <v>1140</v>
+      </c>
+      <c r="F76" s="7">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="6">
+        <v>5</v>
+      </c>
+      <c r="E77" s="11">
+        <v>854</v>
+      </c>
+      <c r="F77" s="7">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="6">
+        <v>5</v>
+      </c>
+      <c r="E78" s="11">
+        <v>801</v>
+      </c>
+      <c r="F78" s="7">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="B79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="1">
+        <v>5</v>
+      </c>
+      <c r="E79" s="8">
+        <v>1100</v>
+      </c>
+      <c r="F79" s="5">
+        <v>44216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>5</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1190</v>
+      </c>
+      <c r="F80" s="5">
+        <v>44217</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1">
+        <v>5</v>
+      </c>
+      <c r="E81" s="8">
+        <v>849</v>
+      </c>
+      <c r="F81" s="5">
+        <v>44217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1">
+        <v>5</v>
+      </c>
+      <c r="E82" s="8">
+        <v>670</v>
+      </c>
+      <c r="F82" s="5">
+        <v>44217</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="6">
+        <v>5</v>
+      </c>
+      <c r="E83" s="11">
+        <v>1170</v>
+      </c>
+      <c r="F83" s="7">
+        <v>44223</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="6">
+        <v>5</v>
+      </c>
+      <c r="E84" s="11">
+        <v>1190</v>
+      </c>
+      <c r="F84" s="7">
+        <v>44224</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="6">
+        <v>5</v>
+      </c>
+      <c r="E85" s="11">
+        <v>1130</v>
+      </c>
+      <c r="F85" s="7">
+        <v>44223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="6">
+        <v>5</v>
+      </c>
+      <c r="E86" s="11">
+        <v>2220</v>
+      </c>
+      <c r="F86" s="7">
+        <v>44223</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="1">
+        <v>5</v>
+      </c>
+      <c r="E87" s="8">
+        <v>673</v>
+      </c>
+      <c r="F87" s="5">
+        <v>44217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="6">
         <v>3</v>
       </c>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="1">
+      <c r="E88" s="11">
+        <v>725</v>
+      </c>
+      <c r="F88" s="7">
+        <v>44237</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="6">
         <v>4</v>
       </c>
-      <c r="E74" s="5">
-        <v>44187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="1">
-        <v>5</v>
-      </c>
-      <c r="E75" s="5">
-        <v>44216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="1">
-        <v>5</v>
-      </c>
-      <c r="E76" s="5">
-        <v>44217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="1">
-        <v>5</v>
-      </c>
-      <c r="E77" s="5">
-        <v>44217</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="1">
-        <v>5</v>
-      </c>
-      <c r="E78" s="5">
-        <v>44217</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="1">
-        <v>5</v>
-      </c>
-      <c r="E79" s="5">
-        <v>44217</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="6">
-        <v>5</v>
-      </c>
-      <c r="E80" s="7">
-        <v>44223</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="6">
-        <v>5</v>
-      </c>
-      <c r="E81" s="7">
-        <v>44223</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="6">
-        <v>5</v>
-      </c>
-      <c r="E82" s="7">
-        <v>44223</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="6">
-        <v>5</v>
-      </c>
-      <c r="E83" s="7">
-        <v>44224</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="6">
-        <v>5</v>
-      </c>
-      <c r="E84" s="7">
-        <v>44225</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" s="6">
-        <v>5</v>
-      </c>
-      <c r="E85" s="7">
-        <v>44225</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="E89" s="11"/>
+      <c r="F89" s="7">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="6">
+        <v>4</v>
+      </c>
+      <c r="E90" s="11"/>
+      <c r="F90" s="7">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="6">
+        <v>4</v>
+      </c>
+      <c r="E91" s="11"/>
+      <c r="F91" s="7">
+        <v>44170</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="6">
-        <v>5</v>
-      </c>
-      <c r="E86" s="7">
-        <v>44230</v>
+      <c r="E92" s="8">
+        <f>SUBTOTAL(109,Tabela1[Peso MB])</f>
+        <v>11786</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A1:XFD60 A61:D61 F61:XFD61 A62:XFD70 A71:D71 F71:XFD71 A72:XFD87 G88:XFD1048576 A92:F1048576">
     <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C86">
+  <conditionalFormatting sqref="C2:C92">
     <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A86">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"CC"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A91">
+    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>